<commit_message>
attachments added fixed bugs
</commit_message>
<xml_diff>
--- a/quickmailer/bin/Debug/list.xlsx
+++ b/quickmailer/bin/Debug/list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\BSUIR\4 sem\КСИС\Lab4\quickmailer\quickmailer\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\ксис\4\quickmailer\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622B9E63-E141-4C34-BDBB-A2167DD4D9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD85794-76F1-4878-AE28-71ED66C05F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26370" yWindow="10410" windowWidth="11730" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,17 +386,17 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="0.140625" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>